<commit_message>
Everything applied to our own dataset
</commit_message>
<xml_diff>
--- a/trajectory_probs.xlsx
+++ b/trajectory_probs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BramUser\Desktop\Studie + Tilburg\DSAI\Algorithms for Geovisualization\algorithm_repository\Flow-Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977AC7D3-4835-40D7-9235-BDC47E0ED8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59ED215-3BE5-4CAE-82AB-5F2FD87B27FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,16 +967,16 @@
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="L8" s="1">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="15">
         <v>0</v>

</xml_diff>